<commit_message>
Retry Analyzer and Data provider topics are covered!!
</commit_message>
<xml_diff>
--- a/sdet-14/Data/testdata.xlsx
+++ b/sdet-14/Data/testdata.xlsx
@@ -4,16 +4,17 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18520" windowHeight="5830"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15690" windowHeight="6075" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="org" sheetId="1" r:id="rId1"/>
-    <sheet name="contact" sheetId="2" r:id="rId2"/>
-    <sheet name="po" sheetId="3" r:id="rId3"/>
-    <sheet name="product" sheetId="4" r:id="rId4"/>
+    <sheet name="CreateMultipleOrg" sheetId="5" r:id="rId2"/>
+    <sheet name="contact" sheetId="2" r:id="rId3"/>
+    <sheet name="po" sheetId="3" r:id="rId4"/>
+    <sheet name="product" sheetId="4" r:id="rId5"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1"/>
+  <oleSize ref="A1:P18"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -23,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="49">
   <si>
     <t>TC_ID</t>
   </si>
@@ -143,19 +144,52 @@
   </si>
   <si>
     <t>Type</t>
+  </si>
+  <si>
+    <t>OrganizationName</t>
+  </si>
+  <si>
+    <t>Industry</t>
+  </si>
+  <si>
+    <t>Phone</t>
+  </si>
+  <si>
+    <t>Amazon</t>
+  </si>
+  <si>
+    <t>Technology</t>
+  </si>
+  <si>
+    <t>ICICI</t>
+  </si>
+  <si>
+    <t>1234567</t>
+  </si>
+  <si>
+    <t>678904</t>
+  </si>
+  <si>
+    <t>4765785</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF222222"/>
+      <name val="Consolas"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="3">
@@ -199,7 +233,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -210,6 +244,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -492,18 +528,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="27.81640625" customWidth="1"/>
-    <col min="3" max="3" width="18.26953125" customWidth="1"/>
-    <col min="4" max="4" width="15.26953125" customWidth="1"/>
+    <col min="2" max="2" width="27.85546875" customWidth="1"/>
+    <col min="3" max="3" width="18.28515625" customWidth="1"/>
+    <col min="4" max="4" width="15.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -515,7 +551,7 @@
       </c>
       <c r="D1" s="3"/>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>2</v>
       </c>
@@ -527,7 +563,7 @@
       </c>
       <c r="D2" s="4"/>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>0</v>
       </c>
@@ -541,7 +577,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>5</v>
       </c>
@@ -555,7 +591,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>0</v>
       </c>
@@ -569,7 +605,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>7</v>
       </c>
@@ -590,20 +626,84 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18.5703125" customWidth="1"/>
+    <col min="2" max="2" width="12.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>48</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="28.54296875" customWidth="1"/>
-    <col min="3" max="3" width="16.1796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.5703125" customWidth="1"/>
+    <col min="3" max="3" width="16.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="23" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -617,7 +717,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -628,10 +728,10 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B3" s="2"/>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>0</v>
       </c>
@@ -645,7 +745,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -664,7 +764,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I2"/>
   <sheetViews>
@@ -672,18 +772,18 @@
       <selection activeCell="B13" sqref="B11:B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="18.90625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.1796875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.54296875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.1796875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.453125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.7265625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.1796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -712,7 +812,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>2</v>
       </c>
@@ -747,7 +847,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D2"/>
   <sheetViews>
@@ -755,14 +855,14 @@
       <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="43.81640625" customWidth="1"/>
+    <col min="2" max="2" width="43.85546875" customWidth="1"/>
     <col min="3" max="3" width="52" customWidth="1"/>
-    <col min="4" max="4" width="45.7265625" customWidth="1"/>
+    <col min="4" max="4" width="45.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -774,7 +874,7 @@
       </c>
       <c r="D1" s="1"/>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>7</v>
       </c>

</xml_diff>